<commit_message>
parametric bootstrap from Trosvik et al 2012 poles
</commit_message>
<xml_diff>
--- a/data/VGPs_NAM/16.xlsx
+++ b/data/VGPs_NAM/16.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="70">
   <si>
     <t>Study level data</t>
   </si>
@@ -116,6 +116,9 @@
     <t>Stoddard Mountain laccolith</t>
   </si>
   <si>
+    <t>uniform</t>
+  </si>
+  <si>
     <t>plutonic</t>
   </si>
   <si>
@@ -158,9 +161,6 @@
   </si>
   <si>
     <t>SMI</t>
-  </si>
-  <si>
-    <t>linear</t>
   </si>
   <si>
     <t>y</t>
@@ -325,9 +325,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -356,12 +354,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border/>
     <border>
       <left/>
@@ -369,25 +367,11 @@
       <top/>
       <bottom/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -421,32 +405,24 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -469,11 +445,8 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -836,55 +809,61 @@
       <c r="C3" s="12">
         <v>246.6</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="13">
         <v>19.0</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14">
+      <c r="E3" s="14">
+        <v>351.1</v>
+      </c>
+      <c r="F3" s="14">
+        <v>57.8</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16">
+        <v>3.7</v>
+      </c>
+      <c r="I3" s="12">
+        <v>-82.9</v>
+      </c>
+      <c r="J3" s="12">
+        <v>346.2</v>
+      </c>
+      <c r="K3" s="16">
         <v>82.2</v>
       </c>
-      <c r="H3" s="14">
-        <v>3.7</v>
-      </c>
-      <c r="I3" s="15">
-        <v>-82.9</v>
-      </c>
-      <c r="J3" s="15">
-        <v>346.2</v>
-      </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="20">
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="17">
         <v>20.0</v>
       </c>
-      <c r="R3" s="20">
+      <c r="R3" s="17">
         <v>22.0</v>
       </c>
-      <c r="S3" s="18"/>
-      <c r="T3" s="14" t="s">
+      <c r="S3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="20">
+      <c r="T3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U3" s="17">
         <v>5.0</v>
       </c>
-      <c r="V3" s="19"/>
-      <c r="W3" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="22" t="s">
+      <c r="V3" s="15"/>
+      <c r="W3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="Z3" s="18"/>
-      <c r="AA3" s="23"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="21"/>
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
-      <c r="AD3" s="24"/>
+      <c r="AD3" s="22"/>
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
     </row>
@@ -924,7 +903,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -968,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>5</v>
@@ -980,13 +959,13 @@
         <v>7</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>11</v>
@@ -1042,67 +1021,59 @@
       <c r="AF6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="26">
+      <c r="A7" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="24">
         <v>37.6</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="24">
         <v>246.6</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="25">
         <v>6.0</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="26">
         <v>340.6</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="26">
         <v>64.6</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="28">
+      <c r="G7" s="27">
+        <v>97.61</v>
+      </c>
+      <c r="H7" s="26">
         <v>6.8</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I7" s="26">
         <v>73.1</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="26">
         <v>-165.3</v>
       </c>
-      <c r="K7" s="28">
-        <v>97.61</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R7" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S7" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U7" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V7" s="31" t="s">
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U7" s="15"/>
+      <c r="V7" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W7" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X7" s="32" t="s">
+      <c r="W7" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X7" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Y7" s="33" t="s">
+      <c r="Y7" s="30" t="s">
         <v>39</v>
       </c>
       <c r="Z7" s="2"/>
@@ -1114,64 +1085,56 @@
       <c r="AF7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="24">
         <v>37.6</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="24">
         <v>246.6</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="25">
         <v>7.0</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="26">
         <v>340.7</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="26">
         <v>60.9</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="28">
+      <c r="G8" s="27">
+        <v>125.73</v>
+      </c>
+      <c r="H8" s="26">
         <v>5.4</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="26">
         <v>74.5</v>
       </c>
-      <c r="J8" s="28">
+      <c r="J8" s="26">
         <v>179.3</v>
       </c>
-      <c r="K8" s="28">
-        <v>125.73</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R8" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S8" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T8" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U8" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V8" s="31" t="s">
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U8" s="15"/>
+      <c r="V8" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W8" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X8" s="32" t="s">
+      <c r="W8" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X8" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y8" s="2"/>
@@ -1184,64 +1147,56 @@
       <c r="AF8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="24">
         <v>37.6</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="24">
         <v>246.6</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="25">
         <v>5.0</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="26">
         <v>348.9</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="26">
         <v>65.7</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="28">
+      <c r="G9" s="27">
+        <v>89.85</v>
+      </c>
+      <c r="H9" s="26">
         <v>8.1</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="26">
         <v>76.8</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="26">
         <v>212.1</v>
       </c>
-      <c r="K9" s="28">
-        <v>89.85</v>
-      </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R9" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S9" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T9" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U9" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V9" s="31" t="s">
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U9" s="15"/>
+      <c r="V9" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W9" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X9" s="32" t="s">
+      <c r="W9" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X9" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y9" s="2"/>
@@ -1254,64 +1209,56 @@
       <c r="AF9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="24">
         <v>37.6</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="24">
         <v>246.6</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="25">
         <v>5.0</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="26">
         <v>357.1</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="26">
         <v>52.2</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="28">
+      <c r="G10" s="27">
+        <v>116.45</v>
+      </c>
+      <c r="H10" s="26">
         <v>7.1</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="26">
         <v>84.7</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="26">
         <v>94.1</v>
       </c>
-      <c r="K10" s="28">
-        <v>116.45</v>
-      </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R10" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S10" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T10" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U10" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V10" s="31" t="s">
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U10" s="15"/>
+      <c r="V10" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W10" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X10" s="32" t="s">
+      <c r="W10" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X10" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y10" s="2"/>
@@ -1324,64 +1271,56 @@
       <c r="AF10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="24">
         <v>37.6</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="24">
         <v>246.6</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="25">
         <v>6.0</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="26">
         <v>0.9</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="26">
         <v>54.8</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="28">
+      <c r="G11" s="27">
+        <v>97.05</v>
+      </c>
+      <c r="H11" s="26">
         <v>6.8</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I11" s="26">
         <v>87.6</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="26">
         <v>47.8</v>
       </c>
-      <c r="K11" s="28">
-        <v>97.05</v>
-      </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R11" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S11" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T11" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U11" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V11" s="31" t="s">
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U11" s="15"/>
+      <c r="V11" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W11" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X11" s="32" t="s">
+      <c r="W11" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X11" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y11" s="2"/>
@@ -1394,64 +1333,56 @@
       <c r="AF11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="24">
         <v>37.6</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="24">
         <v>246.6</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="25">
         <v>6.0</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="26">
         <v>179.3</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="26">
         <v>-68.9</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="28">
+      <c r="G12" s="27">
+        <v>73.95</v>
+      </c>
+      <c r="H12" s="26">
         <v>7.8</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="26">
         <v>-75.1</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="26">
         <v>64.9</v>
       </c>
-      <c r="K12" s="28">
-        <v>73.95</v>
-      </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R12" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S12" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T12" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U12" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V12" s="31" t="s">
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U12" s="15"/>
+      <c r="V12" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W12" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X12" s="32" t="s">
+      <c r="W12" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X12" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y12" s="2"/>
@@ -1464,67 +1395,59 @@
       <c r="AF12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="24">
         <v>37.6</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="24">
         <v>246.6</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="25">
         <v>6.0</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="26">
         <v>181.2</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="26">
         <v>21.1</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="28">
+      <c r="G13" s="27">
+        <v>20.7</v>
+      </c>
+      <c r="H13" s="26">
         <v>15.1</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="26">
         <v>-41.5</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="26">
         <v>-114.9</v>
       </c>
-      <c r="K13" s="28">
-        <v>20.7</v>
-      </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R13" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S13" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U13" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V13" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="W13" s="31" t="s">
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="X13" s="32" t="s">
+      <c r="U13" s="15"/>
+      <c r="V13" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="W13" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X13" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Y13" s="34" t="s">
+      <c r="Y13" s="31" t="s">
         <v>46</v>
       </c>
       <c r="Z13" s="2"/>
@@ -1536,67 +1459,59 @@
       <c r="AF13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="24">
         <v>37.6</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="24">
         <v>246.6</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="25">
         <v>5.0</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="26">
         <v>180.6</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="26">
         <v>13.0</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="28">
+      <c r="G14" s="27">
+        <v>37.15</v>
+      </c>
+      <c r="H14" s="26">
         <v>12.7</v>
       </c>
-      <c r="I14" s="28">
+      <c r="I14" s="26">
         <v>-45.8</v>
       </c>
-      <c r="J14" s="28">
+      <c r="J14" s="26">
         <v>-114.2</v>
       </c>
-      <c r="K14" s="28">
-        <v>37.15</v>
-      </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R14" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S14" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T14" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U14" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V14" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="W14" s="31" t="s">
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="X14" s="32" t="s">
+      <c r="U14" s="15"/>
+      <c r="V14" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="W14" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X14" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Y14" s="34" t="s">
+      <c r="Y14" s="31" t="s">
         <v>46</v>
       </c>
       <c r="Z14" s="2"/>
@@ -1608,67 +1523,59 @@
       <c r="AF14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="24">
         <v>37.6</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="24">
         <v>246.6</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="25">
         <v>6.0</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="26">
         <v>182.7</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="26">
         <v>12.8</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="28">
+      <c r="G15" s="27">
+        <v>60.88</v>
+      </c>
+      <c r="H15" s="26">
         <v>8.7</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I15" s="26">
         <v>-45.9</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="26">
         <v>-117.3</v>
       </c>
-      <c r="K15" s="28">
-        <v>60.88</v>
-      </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R15" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S15" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T15" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U15" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V15" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="W15" s="31" t="s">
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="X15" s="32" t="s">
+      <c r="U15" s="15"/>
+      <c r="V15" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="W15" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X15" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Y15" s="34" t="s">
+      <c r="Y15" s="31" t="s">
         <v>46</v>
       </c>
       <c r="Z15" s="2"/>
@@ -1680,67 +1587,59 @@
       <c r="AF15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="24">
         <v>37.6</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="24">
         <v>246.6</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="25">
         <v>6.0</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="26">
         <v>193.2</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="26">
         <v>4.8</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="28">
+      <c r="G16" s="27">
+        <v>42.54</v>
+      </c>
+      <c r="H16" s="26">
         <v>10.4</v>
       </c>
-      <c r="I16" s="28">
+      <c r="I16" s="26">
         <v>-48.2</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="26">
         <v>-133.4</v>
       </c>
-      <c r="K16" s="28">
-        <v>42.54</v>
-      </c>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R16" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S16" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T16" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U16" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V16" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="W16" s="31" t="s">
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="X16" s="32" t="s">
+      <c r="U16" s="15"/>
+      <c r="V16" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="W16" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X16" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Y16" s="34" t="s">
+      <c r="Y16" s="31" t="s">
         <v>46</v>
       </c>
       <c r="Z16" s="2"/>
@@ -1752,64 +1651,56 @@
       <c r="AF16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="24">
         <v>37.6</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="24">
         <v>246.6</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="25">
         <v>6.0</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="26">
         <v>336.6</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="26">
         <v>46.9</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="28">
+      <c r="G17" s="27">
+        <v>51.97</v>
+      </c>
+      <c r="H17" s="26">
         <v>9.4</v>
       </c>
-      <c r="I17" s="28">
+      <c r="I17" s="26">
         <v>68.3</v>
       </c>
-      <c r="J17" s="28">
+      <c r="J17" s="26">
         <v>137.8</v>
       </c>
-      <c r="K17" s="28">
-        <v>51.97</v>
-      </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R17" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S17" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T17" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U17" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V17" s="31" t="s">
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U17" s="15"/>
+      <c r="V17" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W17" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X17" s="32" t="s">
+      <c r="W17" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X17" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y17" s="2"/>
@@ -1822,64 +1713,56 @@
       <c r="AF17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="26">
+      <c r="B18" s="24">
         <v>37.6</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="24">
         <v>246.6</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="25">
         <v>4.0</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="26">
         <v>344.5</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="26">
         <v>48.4</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="28">
+      <c r="G18" s="27">
+        <v>287.87</v>
+      </c>
+      <c r="H18" s="26">
         <v>5.4</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="26">
         <v>74.7</v>
       </c>
-      <c r="J18" s="28">
+      <c r="J18" s="26">
         <v>124.2</v>
       </c>
-      <c r="K18" s="28">
-        <v>287.87</v>
-      </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R18" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S18" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T18" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U18" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V18" s="31" t="s">
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U18" s="15"/>
+      <c r="V18" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W18" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X18" s="32" t="s">
+      <c r="W18" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X18" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y18" s="2"/>
@@ -1892,64 +1775,56 @@
       <c r="AF18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="24">
         <v>37.6</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="24">
         <v>246.6</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="25">
         <v>5.0</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="26">
         <v>350.3</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="26">
         <v>51.1</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="28">
+      <c r="G19" s="27">
+        <v>116.36</v>
+      </c>
+      <c r="H19" s="26">
         <v>7.1</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I19" s="26">
         <v>80.2</v>
       </c>
-      <c r="J19" s="28">
+      <c r="J19" s="26">
         <v>115.3</v>
       </c>
-      <c r="K19" s="28">
-        <v>116.36</v>
-      </c>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R19" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S19" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T19" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U19" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V19" s="31" t="s">
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U19" s="15"/>
+      <c r="V19" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W19" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X19" s="32" t="s">
+      <c r="W19" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X19" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y19" s="2"/>
@@ -1962,64 +1837,56 @@
       <c r="AF19" s="2"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="24">
         <v>37.6</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="24">
         <v>246.6</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="25">
         <v>6.0</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="26">
         <v>349.2</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="26">
         <v>55.4</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="28">
+      <c r="G20" s="27">
+        <v>118.2</v>
+      </c>
+      <c r="H20" s="26">
         <v>4.9</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I20" s="26">
         <v>81.2</v>
       </c>
-      <c r="J20" s="28">
+      <c r="J20" s="26">
         <v>140.1</v>
       </c>
-      <c r="K20" s="28">
-        <v>118.2</v>
-      </c>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R20" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S20" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T20" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U20" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V20" s="31" t="s">
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U20" s="15"/>
+      <c r="V20" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W20" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X20" s="32" t="s">
+      <c r="W20" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X20" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y20" s="2"/>
@@ -2032,64 +1899,56 @@
       <c r="AF20" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B21" s="24">
         <v>37.6</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="24">
         <v>246.6</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="25">
         <v>6.0</v>
       </c>
-      <c r="E21" s="28">
+      <c r="E21" s="26">
         <v>349.6</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="26">
         <v>51.0</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="28">
+      <c r="G21" s="27">
+        <v>33.56</v>
+      </c>
+      <c r="H21" s="26">
         <v>11.7</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I21" s="26">
         <v>79.7</v>
       </c>
-      <c r="J21" s="28">
+      <c r="J21" s="26">
         <v>125.3</v>
       </c>
-      <c r="K21" s="28">
-        <v>33.56</v>
-      </c>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R21" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S21" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T21" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U21" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V21" s="31" t="s">
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U21" s="15"/>
+      <c r="V21" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W21" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X21" s="32" t="s">
+      <c r="W21" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X21" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y21" s="2"/>
@@ -2102,64 +1961,56 @@
       <c r="AF21" s="2"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="26">
+      <c r="B22" s="24">
         <v>37.6</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="24">
         <v>246.6</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="25">
         <v>5.0</v>
       </c>
-      <c r="E22" s="28">
+      <c r="E22" s="26">
         <v>10.7</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="26">
         <v>49.5</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="28">
+      <c r="G22" s="27">
+        <v>139.79</v>
+      </c>
+      <c r="H22" s="26">
         <v>6.5</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I22" s="26">
         <v>78.6</v>
       </c>
-      <c r="J22" s="28">
+      <c r="J22" s="26">
         <v>10.3</v>
       </c>
-      <c r="K22" s="28">
-        <v>139.79</v>
-      </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R22" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S22" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T22" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U22" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V22" s="31" t="s">
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U22" s="15"/>
+      <c r="V22" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W22" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X22" s="32" t="s">
+      <c r="W22" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X22" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y22" s="2"/>
@@ -2172,67 +2023,59 @@
       <c r="AF22" s="2"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="26">
+      <c r="B23" s="24">
         <v>37.6</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="24">
         <v>246.6</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="25">
         <v>7.0</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E23" s="26">
         <v>147.1</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="26">
         <v>-73.1</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="28">
+      <c r="G23" s="27">
+        <v>78.69</v>
+      </c>
+      <c r="H23" s="26">
         <v>6.9</v>
       </c>
-      <c r="I23" s="28">
+      <c r="I23" s="26">
         <v>-60.0</v>
       </c>
-      <c r="J23" s="28">
+      <c r="J23" s="26">
         <v>32.4</v>
       </c>
-      <c r="K23" s="28">
-        <v>78.69</v>
-      </c>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R23" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S23" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T23" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U23" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V23" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="W23" s="31" t="s">
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="X23" s="32" t="s">
+      <c r="U23" s="15"/>
+      <c r="V23" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="W23" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X23" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Y23" s="34" t="s">
+      <c r="Y23" s="31" t="s">
         <v>46</v>
       </c>
       <c r="Z23" s="2"/>
@@ -2244,67 +2087,59 @@
       <c r="AF23" s="2"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="26">
+      <c r="B24" s="24">
         <v>37.6</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="24">
         <v>246.6</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D24" s="25">
         <v>4.0</v>
       </c>
-      <c r="E24" s="28">
+      <c r="E24" s="26">
         <v>181.5</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="26">
         <v>-12.3</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="28">
+      <c r="G24" s="27">
+        <v>32.85</v>
+      </c>
+      <c r="H24" s="26">
         <v>16.3</v>
       </c>
-      <c r="I24" s="28">
+      <c r="I24" s="26">
         <v>-58.7</v>
       </c>
-      <c r="J24" s="28">
+      <c r="J24" s="26">
         <v>-116.3</v>
       </c>
-      <c r="K24" s="28">
-        <v>32.85</v>
-      </c>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R24" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S24" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T24" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U24" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V24" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="W24" s="31" t="s">
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="X24" s="32" t="s">
+      <c r="U24" s="15"/>
+      <c r="V24" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="W24" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X24" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Y24" s="34" t="s">
+      <c r="Y24" s="31" t="s">
         <v>46</v>
       </c>
       <c r="Z24" s="2"/>
@@ -2316,64 +2151,56 @@
       <c r="AF24" s="2"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="26">
+      <c r="B25" s="24">
         <v>37.6</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="24">
         <v>246.6</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="25">
         <v>6.0</v>
       </c>
-      <c r="E25" s="28">
+      <c r="E25" s="26">
         <v>349.3</v>
       </c>
-      <c r="F25" s="28">
+      <c r="F25" s="26">
         <v>55.7</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="28">
+      <c r="G25" s="27">
+        <v>104.26</v>
+      </c>
+      <c r="H25" s="26">
         <v>6.6</v>
       </c>
-      <c r="I25" s="28">
+      <c r="I25" s="26">
         <v>81.3</v>
       </c>
-      <c r="J25" s="28">
+      <c r="J25" s="26">
         <v>151.2</v>
       </c>
-      <c r="K25" s="28">
-        <v>104.26</v>
-      </c>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R25" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S25" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T25" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U25" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V25" s="31" t="s">
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U25" s="15"/>
+      <c r="V25" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W25" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X25" s="32" t="s">
+      <c r="W25" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X25" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y25" s="2"/>
@@ -2386,64 +2213,56 @@
       <c r="AF25" s="2"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="26">
+      <c r="B26" s="24">
         <v>37.6</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="24">
         <v>246.6</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D26" s="25">
         <v>5.0</v>
       </c>
-      <c r="E26" s="28">
+      <c r="E26" s="26">
         <v>358.1</v>
       </c>
-      <c r="F26" s="28">
+      <c r="F26" s="26">
         <v>55.2</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="28">
+      <c r="G26" s="27">
+        <v>93.06</v>
+      </c>
+      <c r="H26" s="26">
         <v>8.0</v>
       </c>
-      <c r="I26" s="28">
+      <c r="I26" s="26">
         <v>87.6</v>
       </c>
-      <c r="J26" s="28">
+      <c r="J26" s="26">
         <v>108.2</v>
       </c>
-      <c r="K26" s="28">
-        <v>93.06</v>
-      </c>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R26" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S26" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T26" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U26" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V26" s="31" t="s">
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U26" s="15"/>
+      <c r="V26" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W26" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X26" s="32" t="s">
+      <c r="W26" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X26" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y26" s="2"/>
@@ -2456,64 +2275,56 @@
       <c r="AF26" s="2"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="26">
+      <c r="B27" s="24">
         <v>37.6</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="24">
         <v>246.6</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D27" s="25">
         <v>6.0</v>
       </c>
-      <c r="E27" s="28">
+      <c r="E27" s="26">
         <v>354.8</v>
       </c>
-      <c r="F27" s="28">
+      <c r="F27" s="26">
         <v>58.8</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="28">
+      <c r="G27" s="27">
+        <v>159.46</v>
+      </c>
+      <c r="H27" s="26">
         <v>5.3</v>
       </c>
-      <c r="I27" s="28">
+      <c r="I27" s="26">
         <v>85.5</v>
       </c>
-      <c r="J27" s="28">
+      <c r="J27" s="26">
         <v>184.4</v>
       </c>
-      <c r="K27" s="28">
-        <v>159.46</v>
-      </c>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R27" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S27" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T27" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U27" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V27" s="31" t="s">
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U27" s="15"/>
+      <c r="V27" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W27" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X27" s="32" t="s">
+      <c r="W27" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X27" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y27" s="2"/>
@@ -2526,64 +2337,56 @@
       <c r="AF27" s="2"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="26">
+      <c r="B28" s="24">
         <v>37.6</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="24">
         <v>246.6</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D28" s="25">
         <v>5.0</v>
       </c>
-      <c r="E28" s="28">
+      <c r="E28" s="26">
         <v>349.1</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28" s="26">
         <v>55.9</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="28">
+      <c r="G28" s="27">
+        <v>197.95</v>
+      </c>
+      <c r="H28" s="26">
         <v>5.5</v>
       </c>
-      <c r="I28" s="28">
+      <c r="I28" s="26">
         <v>81.2</v>
       </c>
-      <c r="J28" s="28">
+      <c r="J28" s="26">
         <v>152.9</v>
       </c>
-      <c r="K28" s="28">
-        <v>197.95</v>
-      </c>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R28" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S28" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T28" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U28" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V28" s="31" t="s">
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U28" s="15"/>
+      <c r="V28" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W28" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X28" s="32" t="s">
+      <c r="W28" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X28" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y28" s="2"/>
@@ -2596,64 +2399,56 @@
       <c r="AF28" s="2"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="26">
+      <c r="B29" s="24">
         <v>37.6</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="24">
         <v>246.6</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="25">
         <v>6.0</v>
       </c>
-      <c r="E29" s="28">
+      <c r="E29" s="26">
         <v>355.0</v>
       </c>
-      <c r="F29" s="28">
+      <c r="F29" s="26">
         <v>57.8</v>
       </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="28">
+      <c r="G29" s="27">
+        <v>376.1</v>
+      </c>
+      <c r="H29" s="26">
         <v>3.5</v>
       </c>
-      <c r="I29" s="28">
+      <c r="I29" s="26">
         <v>86.0</v>
       </c>
-      <c r="J29" s="28">
+      <c r="J29" s="26">
         <v>171.0</v>
       </c>
-      <c r="K29" s="28">
-        <v>376.1</v>
-      </c>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R29" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S29" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T29" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U29" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V29" s="31" t="s">
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U29" s="15"/>
+      <c r="V29" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W29" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X29" s="32" t="s">
+      <c r="W29" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X29" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y29" s="2"/>
@@ -2666,67 +2461,59 @@
       <c r="AF29" s="2"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="26">
+      <c r="B30" s="24">
         <v>37.6</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="24">
         <v>246.6</v>
       </c>
-      <c r="D30" s="27">
+      <c r="D30" s="25">
         <v>6.0</v>
       </c>
-      <c r="E30" s="28">
+      <c r="E30" s="26">
         <v>172.4</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F30" s="26">
         <v>-8.6</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="28">
+      <c r="G30" s="27">
+        <v>55.06</v>
+      </c>
+      <c r="H30" s="26">
         <v>9.1</v>
       </c>
-      <c r="I30" s="28">
+      <c r="I30" s="26">
         <v>-56.1</v>
       </c>
-      <c r="J30" s="28">
+      <c r="J30" s="26">
         <v>-99.7</v>
       </c>
-      <c r="K30" s="28">
-        <v>55.06</v>
-      </c>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R30" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S30" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T30" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U30" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V30" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="W30" s="31" t="s">
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="X30" s="32" t="s">
+      <c r="U30" s="15"/>
+      <c r="V30" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="W30" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X30" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Y30" s="34" t="s">
+      <c r="Y30" s="31" t="s">
         <v>46</v>
       </c>
       <c r="Z30" s="2"/>
@@ -2738,67 +2525,59 @@
       <c r="AF30" s="2"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="26">
+      <c r="B31" s="24">
         <v>37.6</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="24">
         <v>246.6</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D31" s="25">
         <v>5.0</v>
       </c>
-      <c r="E31" s="28">
+      <c r="E31" s="26">
         <v>187.5</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="26">
         <v>11.4</v>
       </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="28">
+      <c r="G31" s="27">
+        <v>71.0093</v>
+      </c>
+      <c r="H31" s="26">
         <v>9.1</v>
       </c>
-      <c r="I31" s="28">
+      <c r="I31" s="26">
         <v>-46.0</v>
       </c>
-      <c r="J31" s="28">
+      <c r="J31" s="26">
         <v>-128.5</v>
       </c>
-      <c r="K31" s="28">
-        <v>71.0093</v>
-      </c>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R31" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S31" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T31" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U31" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V31" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="W31" s="31" t="s">
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="X31" s="32" t="s">
+      <c r="U31" s="15"/>
+      <c r="V31" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="W31" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X31" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Y31" s="34" t="s">
+      <c r="Y31" s="31" t="s">
         <v>46</v>
       </c>
       <c r="Z31" s="2"/>
@@ -2810,67 +2589,59 @@
       <c r="AF31" s="2"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="26">
+      <c r="B32" s="24">
         <v>37.6</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="24">
         <v>246.6</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D32" s="25">
         <v>5.0</v>
       </c>
-      <c r="E32" s="28">
+      <c r="E32" s="26">
         <v>158.3</v>
       </c>
-      <c r="F32" s="28">
+      <c r="F32" s="26">
         <v>3.8</v>
       </c>
-      <c r="G32" s="2"/>
-      <c r="H32" s="28">
+      <c r="G32" s="27">
+        <v>179.9127</v>
+      </c>
+      <c r="H32" s="26">
         <v>5.7</v>
       </c>
-      <c r="I32" s="28">
+      <c r="I32" s="26">
         <v>-45.6</v>
       </c>
-      <c r="J32" s="28">
+      <c r="J32" s="26">
         <v>-85.9</v>
       </c>
-      <c r="K32" s="28">
-        <v>179.9127</v>
-      </c>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R32" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S32" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T32" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U32" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V32" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="W32" s="31" t="s">
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="X32" s="32" t="s">
+      <c r="U32" s="15"/>
+      <c r="V32" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="W32" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X32" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Y32" s="34" t="s">
+      <c r="Y32" s="31" t="s">
         <v>46</v>
       </c>
       <c r="Z32" s="2"/>
@@ -2882,67 +2653,59 @@
       <c r="AF32" s="2"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="26">
+      <c r="B33" s="24">
         <v>37.6</v>
       </c>
-      <c r="C33" s="26">
+      <c r="C33" s="24">
         <v>246.6</v>
       </c>
-      <c r="D33" s="27">
+      <c r="D33" s="25">
         <v>5.0</v>
       </c>
-      <c r="E33" s="28">
+      <c r="E33" s="26">
         <v>174.7</v>
       </c>
-      <c r="F33" s="28">
+      <c r="F33" s="26">
         <v>-9.6</v>
       </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="28">
+      <c r="G33" s="27">
+        <v>35.3153</v>
+      </c>
+      <c r="H33" s="26">
         <v>13.1</v>
       </c>
-      <c r="I33" s="28">
+      <c r="I33" s="26">
         <v>-56.8</v>
       </c>
-      <c r="J33" s="28">
+      <c r="J33" s="26">
         <v>-108.0</v>
       </c>
-      <c r="K33" s="28">
-        <v>35.3153</v>
-      </c>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R33" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S33" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T33" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U33" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V33" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="W33" s="31" t="s">
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="X33" s="32" t="s">
+      <c r="U33" s="15"/>
+      <c r="V33" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="W33" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X33" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Y33" s="34" t="s">
+      <c r="Y33" s="31" t="s">
         <v>46</v>
       </c>
       <c r="Z33" s="2"/>
@@ -2954,64 +2717,56 @@
       <c r="AF33" s="2"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="26">
+      <c r="B34" s="24">
         <v>37.6</v>
       </c>
-      <c r="C34" s="26">
+      <c r="C34" s="24">
         <v>246.6</v>
       </c>
-      <c r="D34" s="27">
+      <c r="D34" s="25">
         <v>7.0</v>
       </c>
-      <c r="E34" s="28">
+      <c r="E34" s="26">
         <v>177.8</v>
       </c>
-      <c r="F34" s="28">
+      <c r="F34" s="26">
         <v>-30.9</v>
       </c>
-      <c r="G34" s="2"/>
-      <c r="H34" s="28">
+      <c r="G34" s="27">
+        <v>52.6411</v>
+      </c>
+      <c r="H34" s="26">
         <v>8.4</v>
       </c>
-      <c r="I34" s="28">
+      <c r="I34" s="26">
         <v>-68.9</v>
       </c>
-      <c r="J34" s="28">
+      <c r="J34" s="26">
         <v>-111.9</v>
       </c>
-      <c r="K34" s="28">
-        <v>52.6411</v>
-      </c>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R34" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S34" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T34" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U34" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V34" s="31" t="s">
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
+      <c r="T34" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U34" s="15"/>
+      <c r="V34" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W34" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X34" s="32" t="s">
+      <c r="W34" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X34" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y34" s="2"/>
@@ -3024,67 +2779,59 @@
       <c r="AF34" s="2"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="26">
+      <c r="B35" s="24">
         <v>37.6</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="24">
         <v>246.6</v>
       </c>
-      <c r="D35" s="27">
+      <c r="D35" s="25">
         <v>4.0</v>
       </c>
-      <c r="E35" s="28">
+      <c r="E35" s="26">
         <v>174.1</v>
       </c>
-      <c r="F35" s="28">
+      <c r="F35" s="26">
         <v>3.4</v>
       </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="28">
+      <c r="G35" s="27">
+        <v>163.6567</v>
+      </c>
+      <c r="H35" s="26">
         <v>7.2</v>
       </c>
-      <c r="I35" s="28">
+      <c r="I35" s="26">
         <v>-50.3</v>
       </c>
-      <c r="J35" s="28">
+      <c r="J35" s="26">
         <v>-108.6</v>
       </c>
-      <c r="K35" s="28">
-        <v>163.6567</v>
-      </c>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="20"/>
-      <c r="Q35" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R35" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S35" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T35" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U35" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V35" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="W35" s="31" t="s">
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="X35" s="32" t="s">
+      <c r="U35" s="15"/>
+      <c r="V35" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="W35" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X35" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Y35" s="34" t="s">
+      <c r="Y35" s="31" t="s">
         <v>46</v>
       </c>
       <c r="Z35" s="2"/>
@@ -3096,64 +2843,56 @@
       <c r="AF35" s="2"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="26">
+      <c r="B36" s="24">
         <v>37.6</v>
       </c>
-      <c r="C36" s="26">
+      <c r="C36" s="24">
         <v>246.6</v>
       </c>
-      <c r="D36" s="27">
+      <c r="D36" s="25">
         <v>5.0</v>
       </c>
-      <c r="E36" s="28">
+      <c r="E36" s="26">
         <v>358.8</v>
       </c>
-      <c r="F36" s="28">
+      <c r="F36" s="26">
         <v>66.6</v>
       </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="28">
+      <c r="G36" s="27">
+        <v>97.6953</v>
+      </c>
+      <c r="H36" s="26">
         <v>7.8</v>
       </c>
-      <c r="I36" s="28">
+      <c r="I36" s="26">
         <v>78.5</v>
       </c>
-      <c r="J36" s="28">
+      <c r="J36" s="26">
         <v>-121.7</v>
       </c>
-      <c r="K36" s="28">
-        <v>97.6953</v>
-      </c>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="20">
-        <v>20.0</v>
-      </c>
-      <c r="R36" s="20">
-        <v>22.0</v>
-      </c>
-      <c r="S36" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T36" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U36" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="V36" s="31" t="s">
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U36" s="15"/>
+      <c r="V36" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="W36" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X36" s="32" t="s">
+      <c r="W36" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="X36" s="29" t="s">
         <v>38</v>
       </c>
       <c r="Y36" s="2"/>

</xml_diff>